<commit_message>
updated with new data dated 190624
</commit_message>
<xml_diff>
--- a/data/kostra_description.xlsx
+++ b/data/kostra_description.xlsx
@@ -842,8 +842,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100D6442C570680934CB22BA5BC5A092BF3" ma:contentTypeVersion="12" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="d397461c7fbf4fb75751d6c10f41a95f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07626311-5b23-4afe-aa20-cc40db419bd4" xmlns:ns3="d74b2904-cc6e-4260-b9ea-005e83d891d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ab8cf7be5c815422baaa066a5d49f2c7" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100D6442C570680934CB22BA5BC5A092BF3" ma:contentTypeVersion="15" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="f5b76c4a68413fae7c9234b2446bfa6b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07626311-5b23-4afe-aa20-cc40db419bd4" xmlns:ns3="d74b2904-cc6e-4260-b9ea-005e83d891d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac5eb3307540f0e734bb4e2514f51241" ns2:_="" ns3:_="">
     <xsd:import namespace="07626311-5b23-4afe-aa20-cc40db419bd4"/>
     <xsd:import namespace="d74b2904-cc6e-4260-b9ea-005e83d891d2"/>
     <xsd:element name="properties">
@@ -863,6 +863,9 @@
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -913,6 +916,23 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="20" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="22" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1065,10 +1085,25 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07626311-5b23-4afe-aa20-cc40db419bd4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d74b2904-cc6e-4260-b9ea-005e83d891d2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E792D0A-511F-423B-AF5D-F90918489175}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8899C90D-31AC-42E4-89BF-900CD47CFBCF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7274AFD1-8273-4D6A-9299-61D1826BBE2D}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46AD9A0C-BA0E-48B7-92D1-B74AC6665BDC}"/>
 </file>
</xml_diff>